<commit_message>
removed studies that weren't included in meta-analysis
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/catchment_characteristics/Fire_name_Lat_Long.xlsx
+++ b/FireMeta_Rproj/inputs/catchment_characteristics/Fire_name_Lat_Long.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/Studies_Summary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/catchment_characteristics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F1B532-395A-1147-B111-F8708C3564D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2B76BE-63AC-3344-8DD3-3B6DA6D261B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{8C258C6F-044A-E849-9C14-F26FA5F5AA92}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{8C258C6F-044A-E849-9C14-F26FA5F5AA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Temporal Normalization Studies" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
     <t xml:space="preserve">44.578525	</t>
   </si>
   <si>
-    <t>Have_HUC?</t>
-  </si>
-  <si>
     <t>N_Canada</t>
   </si>
   <si>
@@ -893,6 +890,9 @@
   </si>
   <si>
     <t>lnR5</t>
+  </si>
+  <si>
+    <t>Have_HUC</t>
   </si>
 </sst>
 </file>
@@ -1129,9 +1129,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1169,7 +1169,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1275,7 +1275,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1417,7 +1417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1429,7 +1429,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1449,7 +1449,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1458,13 +1458,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -1488,7 +1488,7 @@
         <v>86</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>107</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -1501,10 +1501,10 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1515,10 +1515,10 @@
         <v>37</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>231</v>
       </c>
       <c r="G3">
         <v>61.4</v>
@@ -1542,7 +1542,7 @@
         <v>84</v>
       </c>
       <c r="N3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1553,13 +1553,13 @@
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>231</v>
       </c>
       <c r="G4">
         <v>61.133333</v>
@@ -1583,7 +1583,7 @@
         <v>84</v>
       </c>
       <c r="N4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -1596,10 +1596,10 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1610,13 +1610,13 @@
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="G6">
         <v>34.472966</v>
@@ -1651,13 +1651,13 @@
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="G7">
         <v>34.484966</v>
@@ -1692,13 +1692,13 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="G8">
         <v>34.475085999999997</v>
@@ -1734,10 +1734,10 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="G9">
         <v>35.526656000000003</v>
@@ -1774,10 +1774,10 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -1790,13 +1790,13 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G11">
         <v>40.134566999999997</v>
@@ -1820,7 +1820,7 @@
         <v>89</v>
       </c>
       <c r="N11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1831,10 +1831,10 @@
         <v>28</v>
       </c>
       <c r="E12" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G12">
         <v>40.180112999999999</v>
@@ -1858,7 +1858,7 @@
         <v>89</v>
       </c>
       <c r="N12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1869,10 +1869,10 @@
         <v>29</v>
       </c>
       <c r="E13" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G13">
         <v>40.184012000000003</v>
@@ -1896,7 +1896,7 @@
         <v>89</v>
       </c>
       <c r="N13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1907,10 +1907,10 @@
         <v>30</v>
       </c>
       <c r="E14" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G14" s="6">
         <v>40.157766000000002</v>
@@ -1945,10 +1945,10 @@
         <v>31</v>
       </c>
       <c r="E15" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G15">
         <v>40.200989</v>
@@ -1984,10 +1984,10 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G16">
         <v>40.192393000000003</v>
@@ -2011,7 +2011,7 @@
         <v>89</v>
       </c>
       <c r="N16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -2022,13 +2022,13 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E17" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G17" s="6">
         <v>39.974595000000001</v>
@@ -2052,7 +2052,7 @@
         <v>89</v>
       </c>
       <c r="N17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -2064,10 +2064,10 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G18">
         <v>40.234889000000003</v>
@@ -2102,13 +2102,13 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E19" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G19">
         <v>40.103144999999998</v>
@@ -2132,7 +2132,7 @@
         <v>89</v>
       </c>
       <c r="N19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -2143,13 +2143,13 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E20" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="G20">
         <v>40.071703999999997</v>
@@ -2186,10 +2186,10 @@
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -2201,10 +2201,10 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="G22" s="8">
         <v>44.512949999999996</v>
@@ -2239,13 +2239,13 @@
         <v>40</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E23" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="G23" s="8">
         <v>44.558208</v>
@@ -2282,10 +2282,10 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -2298,13 +2298,13 @@
         <v>41</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E25" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="G25">
         <v>49.704340000000002</v>
@@ -2328,7 +2328,7 @@
         <v>89</v>
       </c>
       <c r="N25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -2339,13 +2339,13 @@
         <v>42</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E26" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="G26">
         <v>49.712888</v>
@@ -2369,7 +2369,7 @@
         <v>89</v>
       </c>
       <c r="N26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -2381,10 +2381,10 @@
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="G27">
         <v>49.706719</v>
@@ -2408,7 +2408,7 @@
         <v>89</v>
       </c>
       <c r="N27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -2421,10 +2421,10 @@
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
@@ -2437,13 +2437,13 @@
         <v>44</v>
       </c>
       <c r="D29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G29">
         <v>48.81409</v>
@@ -2478,10 +2478,10 @@
         <v>45</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G30">
         <v>48.80153</v>
@@ -2516,13 +2516,13 @@
         <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G31">
         <v>48.802771999999997</v>
@@ -2557,10 +2557,10 @@
         <v>47</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G32">
         <v>48.688412999999997</v>
@@ -2595,10 +2595,10 @@
         <v>49</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G33">
         <v>48.701411999999998</v>
@@ -2622,7 +2622,7 @@
         <v>88</v>
       </c>
       <c r="N33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -2633,13 +2633,13 @@
         <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G34">
         <v>48.797378000000002</v>
@@ -2674,13 +2674,13 @@
         <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G35">
         <v>48.790458000000001</v>
@@ -2715,13 +2715,13 @@
         <v>51</v>
       </c>
       <c r="D36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G36" s="6">
         <v>48.722610000000003</v>
@@ -2756,7 +2756,7 @@
         <v>11</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -2767,13 +2767,13 @@
         <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G38">
         <v>38.883760000000002</v>
@@ -2788,7 +2788,7 @@
         <v>90</v>
       </c>
       <c r="K38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L38" t="s">
         <v>87</v>
@@ -2797,7 +2797,7 @@
         <v>89</v>
       </c>
       <c r="N38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -2808,10 +2808,10 @@
         <v>79</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G39">
         <v>38.898688999999997</v>
@@ -2826,7 +2826,7 @@
         <v>90</v>
       </c>
       <c r="K39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L39" t="s">
         <v>87</v>
@@ -2835,7 +2835,7 @@
         <v>89</v>
       </c>
       <c r="N39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -2846,13 +2846,13 @@
         <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G40">
         <v>38.958700999999998</v>
@@ -2867,7 +2867,7 @@
         <v>90</v>
       </c>
       <c r="K40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L40" t="s">
         <v>87</v>
@@ -2876,7 +2876,7 @@
         <v>89</v>
       </c>
       <c r="N40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -2887,10 +2887,10 @@
         <v>54</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G41">
         <v>39.000053000000001</v>
@@ -2905,7 +2905,7 @@
         <v>90</v>
       </c>
       <c r="K41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L41" t="s">
         <v>87</v>
@@ -2914,7 +2914,7 @@
         <v>89</v>
       </c>
       <c r="N41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -2927,10 +2927,10 @@
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
@@ -2943,13 +2943,13 @@
         <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E43" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F43" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G43">
         <v>48.418961000000003</v>
@@ -2984,10 +2984,10 @@
         <v>56</v>
       </c>
       <c r="E44" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G44">
         <v>48.422220000000003</v>
@@ -3022,13 +3022,13 @@
         <v>57</v>
       </c>
       <c r="D45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E45" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G45">
         <v>48.54888888</v>
@@ -3063,13 +3063,13 @@
         <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E46" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G46">
         <v>48.525536000000002</v>
@@ -3104,13 +3104,13 @@
         <v>59</v>
       </c>
       <c r="D47" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E47" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F47" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="G47">
         <v>48.635277780000003</v>
@@ -3147,10 +3147,10 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G48" s="12">
         <v>40.033332999999999</v>
@@ -3167,13 +3167,13 @@
         <v>60</v>
       </c>
       <c r="D49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G49" s="5">
         <v>40.039045999999999</v>
@@ -3208,13 +3208,13 @@
         <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G50" s="5">
         <v>40.041668000000001</v>
@@ -3249,13 +3249,13 @@
         <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G51" s="5">
         <v>40.015500000000003</v>
@@ -3290,10 +3290,10 @@
         <v>63</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G52" s="5">
         <v>40.036102999999997</v>
@@ -3317,7 +3317,7 @@
         <v>89</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
@@ -3328,10 +3328,10 @@
         <v>64</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G53">
         <v>40.037790999999999</v>
@@ -3368,10 +3368,10 @@
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G54" s="12">
         <v>40.050263700000002</v>
@@ -3388,13 +3388,13 @@
         <v>60</v>
       </c>
       <c r="D55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G55" s="5">
         <v>40.039045999999999</v>
@@ -3429,13 +3429,13 @@
         <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G56" s="5">
         <v>40.041668000000001</v>
@@ -3470,13 +3470,13 @@
         <v>62</v>
       </c>
       <c r="D57" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G57" s="5">
         <v>40.015500000000003</v>
@@ -3511,10 +3511,10 @@
         <v>63</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G58" s="5">
         <v>40.036102999999997</v>
@@ -3538,7 +3538,7 @@
         <v>89</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -3551,10 +3551,10 @@
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G59" s="12">
         <v>36.095348999999999</v>
@@ -3572,10 +3572,10 @@
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G60">
         <v>34.937945999999997</v>
@@ -3610,13 +3610,13 @@
         <v>65</v>
       </c>
       <c r="D61" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G61">
         <v>34.920959000000003</v>
@@ -3640,7 +3640,7 @@
         <v>88</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -3653,10 +3653,10 @@
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
       <c r="E62" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -3668,10 +3668,10 @@
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G63">
         <v>38.868000000000002</v>
@@ -3695,7 +3695,7 @@
         <v>89</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -3707,10 +3707,10 @@
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G64">
         <v>38.880000000000003</v>
@@ -3743,13 +3743,13 @@
         <v>68</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G65">
         <v>38.878999999999998</v>
@@ -3773,7 +3773,7 @@
         <v>89</v>
       </c>
       <c r="N65" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -3784,13 +3784,13 @@
         <v>69</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G66">
         <v>38.872999999999998</v>
@@ -3814,7 +3814,7 @@
         <v>89</v>
       </c>
       <c r="N66" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -3827,10 +3827,10 @@
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
       <c r="E67" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F67" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>250</v>
       </c>
       <c r="G67" s="18"/>
       <c r="H67" s="18"/>
@@ -3843,13 +3843,13 @@
         <v>71</v>
       </c>
       <c r="D68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E68" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F68" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>250</v>
       </c>
       <c r="G68">
         <v>48.035327000000002</v>
@@ -3884,10 +3884,10 @@
         <v>72</v>
       </c>
       <c r="E69" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F69" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>250</v>
       </c>
       <c r="G69">
         <v>48.021419999999999</v>
@@ -3924,10 +3924,10 @@
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
@@ -3938,10 +3938,10 @@
         <v>73</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G71">
         <v>38.451371999999999</v>
@@ -3965,7 +3965,7 @@
         <v>84</v>
       </c>
       <c r="N71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -3976,13 +3976,13 @@
         <v>74</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G72" s="6">
         <v>38.923563999999999</v>
@@ -4006,7 +4006,7 @@
         <v>84</v>
       </c>
       <c r="N72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -4017,13 +4017,13 @@
         <v>75</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G73">
         <v>38.512031</v>
@@ -4045,7 +4045,7 @@
         <v>84</v>
       </c>
       <c r="N73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -4058,10 +4058,10 @@
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
       <c r="E74" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G74" s="19"/>
       <c r="H74" s="19"/>
@@ -4075,10 +4075,10 @@
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G75">
         <v>40.699423000000003</v>
@@ -4113,13 +4113,13 @@
         <v>77</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G76">
         <v>40.685031000000002</v>
@@ -4143,7 +4143,7 @@
         <v>88</v>
       </c>
       <c r="N76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -4154,13 +4154,13 @@
         <v>78</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G77" s="6">
         <v>40.703249</v>
@@ -4197,10 +4197,10 @@
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
       <c r="E78" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -4212,10 +4212,10 @@
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G79">
         <v>40.699423000000003</v>
@@ -4250,13 +4250,13 @@
         <v>78</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G80">
         <v>40.685031000000002</v>
@@ -4280,7 +4280,7 @@
         <v>88</v>
       </c>
       <c r="N80" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
@@ -4291,13 +4291,13 @@
         <v>77</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G81" s="6">
         <v>40.703249</v>
@@ -4326,241 +4326,241 @@
     </row>
     <row r="82" spans="2:14" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E83" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F83" s="29"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C109" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C110" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C112" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C114" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C117" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C118" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C120" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C123" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C124" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C125" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C126" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C127" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="128" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B128" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E128" s="29" t="s">
         <v>94</v>
@@ -4569,7 +4569,7 @@
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C129" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G129">
         <v>65.156433000000007</v>
@@ -4593,12 +4593,12 @@
         <v>87</v>
       </c>
       <c r="N129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C130" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G130">
         <v>65.159576999999999</v>
@@ -4622,12 +4622,12 @@
         <v>87</v>
       </c>
       <c r="N130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="131" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C131" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G131">
         <v>65.158680000000004</v>
@@ -4651,12 +4651,12 @@
         <v>87</v>
       </c>
       <c r="N131" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C132" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G132">
         <v>65.180338000000006</v>
@@ -4680,15 +4680,15 @@
         <v>87</v>
       </c>
       <c r="N132" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B133" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E133" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F133" s="29"/>
     </row>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C135" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G135">
         <v>34.482937999999997</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C136" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G136">
         <v>34.506217999999997</v>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C137" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G137">
         <v>34.458570999999999</v>
@@ -4798,7 +4798,7 @@
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C138" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G138">
         <v>34.492925</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C140" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G140">
         <v>34.452924000000003</v>
@@ -4876,7 +4876,7 @@
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C141" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G141">
         <v>34.456563000000003</v>
@@ -4902,7 +4902,7 @@
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C142" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G142">
         <v>34.443747000000002</v>
@@ -4928,7 +4928,7 @@
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C143" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G143">
         <v>34.464474000000003</v>
@@ -4954,7 +4954,7 @@
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C144" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G144">
         <v>34.470762999999998</v>
@@ -4980,7 +4980,7 @@
     </row>
     <row r="145" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C145" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G145">
         <v>34.465553</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="146" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C146" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G146">
         <v>34.460483000000004</v>
@@ -5032,7 +5032,7 @@
     </row>
     <row r="147" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C147" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G147">
         <v>34.467247999999998</v>
@@ -5058,16 +5058,16 @@
     </row>
     <row r="148" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B148" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F148" s="29"/>
     </row>
     <row r="149" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I149">
         <v>10.59</v>
@@ -5085,12 +5085,12 @@
         <v>87</v>
       </c>
       <c r="N149" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="150" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C150" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I150">
         <v>8.2899999999999991</v>
@@ -5108,12 +5108,12 @@
         <v>87</v>
       </c>
       <c r="N150" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="151" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C151" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I151">
         <v>3.59</v>
@@ -5131,12 +5131,12 @@
         <v>87</v>
       </c>
       <c r="N151" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="152" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I152">
         <v>8.2100000000000009</v>
@@ -5154,12 +5154,12 @@
         <v>87</v>
       </c>
       <c r="N152" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I153">
         <v>7.13</v>
@@ -5177,12 +5177,12 @@
         <v>87</v>
       </c>
       <c r="N153" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="154" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B154" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E154" s="29" t="s">
         <v>103</v>
@@ -5191,7 +5191,7 @@
     </row>
     <row r="155" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C155" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G155">
         <v>35.173952</v>
@@ -5206,18 +5206,18 @@
         <v>84</v>
       </c>
       <c r="L155" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M155" t="s">
         <v>87</v>
       </c>
       <c r="N155" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="156" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G156">
         <v>35.167361999999997</v>
@@ -5232,18 +5232,18 @@
         <v>84</v>
       </c>
       <c r="L156" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M156" t="s">
         <v>87</v>
       </c>
       <c r="N156" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="157" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C157" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G157">
         <v>35.183095999999999</v>
@@ -5258,18 +5258,18 @@
         <v>84</v>
       </c>
       <c r="L157" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M157" t="s">
         <v>87</v>
       </c>
       <c r="N157" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="158" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C158" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G158">
         <v>35.175843</v>
@@ -5284,18 +5284,18 @@
         <v>84</v>
       </c>
       <c r="L158" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M158" t="s">
         <v>87</v>
       </c>
       <c r="N158" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="159" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C159" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G159">
         <v>35.260796999999997</v>
@@ -5310,18 +5310,18 @@
         <v>84</v>
       </c>
       <c r="L159" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M159" t="s">
         <v>87</v>
       </c>
       <c r="N159" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="160" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C160" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G160">
         <v>35.278956999999998</v>
@@ -5336,18 +5336,18 @@
         <v>84</v>
       </c>
       <c r="L160" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M160" t="s">
         <v>87</v>
       </c>
       <c r="N160" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="161" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C161" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G161">
         <v>35.268053000000002</v>
@@ -5362,18 +5362,18 @@
         <v>84</v>
       </c>
       <c r="L161" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M161" t="s">
         <v>87</v>
       </c>
       <c r="N161" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="162" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C162" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G162">
         <v>35.271836999999998</v>
@@ -5388,28 +5388,28 @@
         <v>84</v>
       </c>
       <c r="L162" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M162" t="s">
         <v>87</v>
       </c>
       <c r="N162" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="163" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B163" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E163" s="17" t="s">
         <v>207</v>
-      </c>
-      <c r="E163" s="17" t="s">
-        <v>208</v>
       </c>
       <c r="F163" s="17"/>
     </row>
     <row r="164" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B164" s="4"/>
       <c r="C164" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E164" s="30"/>
       <c r="F164" s="30"/>
@@ -5426,7 +5426,7 @@
         <v>84</v>
       </c>
       <c r="L164" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M164" t="s">
         <v>84</v>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="165" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C165" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G165">
         <v>35.866700000000002</v>
@@ -5449,7 +5449,7 @@
         <v>84</v>
       </c>
       <c r="L165" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M165" t="s">
         <v>84</v>
@@ -5458,7 +5458,7 @@
     <row r="166" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B166" s="4"/>
       <c r="C166" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E166" s="30"/>
       <c r="F166" s="30"/>
@@ -5475,7 +5475,7 @@
         <v>84</v>
       </c>
       <c r="L166" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M166" t="s">
         <v>84</v>
@@ -5483,70 +5483,70 @@
     </row>
     <row r="167" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B167" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E167" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="E167" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="F167" s="11"/>
     </row>
     <row r="168" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B168" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E168" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F168" s="11"/>
     </row>
     <row r="169" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B169" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E169" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="E169" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="F169" s="11"/>
     </row>
     <row r="170" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B170" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E170" s="11" t="s">
         <v>219</v>
-      </c>
-      <c r="E170" s="11" t="s">
-        <v>220</v>
       </c>
       <c r="F170" s="11"/>
     </row>
     <row r="171" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B171" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E171" s="11" t="s">
         <v>221</v>
-      </c>
-      <c r="E171" s="11" t="s">
-        <v>222</v>
       </c>
       <c r="F171" s="11"/>
     </row>
     <row r="172" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B172" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E172" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F172" s="11"/>
     </row>
     <row r="173" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B173" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E173" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F173" s="11"/>
     </row>
     <row r="174" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B174" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E174" s="13" t="s">
         <v>14</v>
@@ -5555,12 +5555,12 @@
     </row>
     <row r="175" spans="2:14" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B175" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="176" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B176" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E176" s="11" t="s">
         <v>96</v>
@@ -5569,7 +5569,7 @@
     </row>
     <row r="177" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B177" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E177" s="11" t="s">
         <v>97</v>
@@ -5578,7 +5578,7 @@
     </row>
     <row r="178" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B178" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E178" s="11" t="s">
         <v>95</v>

</xml_diff>